<commit_message>
did 3 arrays question today
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="72" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="72" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2095,8 +2095,8 @@
       <c r="B22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>4</v>
+      <c r="C22" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2117,8 +2117,8 @@
       <c r="B24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>4</v>
+      <c r="C24" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2128,8 +2128,8 @@
       <c r="B25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>4</v>
+      <c r="C25" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21">

</xml_diff>

<commit_message>
I did 2 questions today
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="72" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScale="72" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2183,8 +2183,8 @@
       <c r="B30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>4</v>
+      <c r="C30" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2205,8 +2205,8 @@
       <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>4</v>
+      <c r="C32" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">

</xml_diff>

<commit_message>
I understood 3 questions today
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2216,8 +2216,8 @@
       <c r="B33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>4</v>
+      <c r="C33" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">
@@ -2227,8 +2227,8 @@
       <c r="B34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>4</v>
+      <c r="C34" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">

</xml_diff>

<commit_message>
done 26 arrays ques in all time
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1497,7 +1497,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1516,6 +1516,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1530,7 +1536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1558,6 +1564,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1877,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="72" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1910,9 +1919,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="C5" s="11" t="s">
-        <v>464</v>
-      </c>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
@@ -1932,8 +1939,8 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
+      <c r="C7" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -2238,8 +2245,8 @@
       <c r="B35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>4</v>
+      <c r="C35" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">
@@ -2249,8 +2256,8 @@
       <c r="B36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>4</v>
+      <c r="C36" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2260,8 +2267,8 @@
       <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
+      <c r="C37" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
@@ -2271,8 +2278,8 @@
       <c r="B38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>4</v>
+      <c r="C38" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2282,8 +2289,8 @@
       <c r="B39" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>4</v>
+      <c r="C39" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2293,8 +2300,8 @@
       <c r="B40" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>4</v>
+      <c r="C40" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2304,22 +2311,18 @@
       <c r="B41" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
+      <c r="C41" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">
       <c r="B42" s="7"/>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" ht="21">
       <c r="A44" s="8" t="s">

</xml_diff>

<commit_message>
did 2 matrix questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="72" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2331,8 +2331,8 @@
       <c r="B44" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>4</v>
+      <c r="C44" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2364,8 +2364,8 @@
       <c r="B47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>4</v>
+      <c r="C47" s="11" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">

</xml_diff>